<commit_message>
Add TFT LCD codes
</commit_message>
<xml_diff>
--- a/OV7670_PIN MAP.xlsx
+++ b/OV7670_PIN MAP.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>SCL</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -103,6 +103,30 @@
   </si>
   <si>
     <t>1000,0000,0000,0000,0000,00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MISO(RX)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOSI(TX)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D/C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -174,16 +198,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>11122</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>174409</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1399</xdr:rowOff>
+      <xdr:rowOff>164685</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>528293</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>103177</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>16665</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>48749</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -200,84 +224,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2710779" y="1399"/>
+          <a:off x="3548980" y="164685"/>
           <a:ext cx="5916485" cy="3585207"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>553517</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>141243</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2007704" y="3935896"/>
-          <a:ext cx="6576630" cy="1234547"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>52335</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>217140</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="669235" y="3935896"/>
-          <a:ext cx="4067743" cy="3934374"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -552,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D38"/>
+  <dimension ref="A2:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -565,7 +513,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -576,7 +524,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -587,7 +535,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -598,7 +546,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -609,7 +557,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -620,7 +568,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
@@ -631,7 +579,7 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -642,7 +590,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
@@ -653,7 +601,7 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
@@ -664,7 +612,7 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
@@ -675,7 +623,7 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
         <v>16</v>
@@ -686,7 +634,7 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
@@ -697,7 +645,7 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -708,10 +656,53 @@
         <v>13</v>
       </c>
       <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="D15" t="s">
-        <v>16</v>
+      <c r="C17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21">
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
SIMD RTL update & test code
</commit_message>
<xml_diff>
--- a/OV7670_PIN MAP.xlsx
+++ b/OV7670_PIN MAP.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="101">
   <si>
     <t>SCL</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -335,6 +335,98 @@
   </si>
   <si>
     <t>IN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIMD_CS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPIO0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c_D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TFT_D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vcc_sys</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vcc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXCUTE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -342,7 +434,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,8 +490,24 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFF00"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,8 +549,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3300"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -530,6 +662,173 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -539,7 +838,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -607,6 +906,78 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -616,6 +987,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -659,6 +1035,44 @@
         <a:xfrm>
           <a:off x="3548980" y="164685"/>
           <a:ext cx="5916485" cy="3585207"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>500743</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>228599</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>659240</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>178740</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="500743" y="12986656"/>
+          <a:ext cx="7582554" cy="4511255"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -933,10 +1347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Z50"/>
+  <dimension ref="A2:Z80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V44" sqref="V44"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T70" sqref="T70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1902,6 +2316,9 @@
       <c r="U41" s="16" t="s">
         <v>51</v>
       </c>
+      <c r="V41" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="42" spans="4:23" x14ac:dyDescent="0.4">
       <c r="F42" s="17" t="s">
@@ -1976,6 +2393,9 @@
       <c r="U43" s="16" t="s">
         <v>50</v>
       </c>
+      <c r="V43" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="44" spans="4:23" x14ac:dyDescent="0.4">
       <c r="D44" t="s">
@@ -2254,7 +2674,308 @@
       </c>
     </row>
     <row r="50" spans="6:23" ht="18" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="58" spans="6:23" x14ac:dyDescent="0.4">
+      <c r="P58" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q58" s="24"/>
+    </row>
+    <row r="59" spans="6:23" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="60" spans="6:23" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O60" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="P60" s="34">
+        <v>1</v>
+      </c>
+      <c r="Q60" s="35">
+        <v>2</v>
+      </c>
+      <c r="R60" s="30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="6:23" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O61" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="P61" s="36">
+        <v>3</v>
+      </c>
+      <c r="Q61" s="37">
+        <v>4</v>
+      </c>
+      <c r="R61" s="31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="6:23" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O62" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="P62" s="36">
+        <v>5</v>
+      </c>
+      <c r="Q62" s="37">
+        <v>6</v>
+      </c>
+      <c r="R62" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="W62" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="63" spans="6:23" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O63" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="P63" s="36">
+        <v>7</v>
+      </c>
+      <c r="Q63" s="37">
+        <v>8</v>
+      </c>
+      <c r="R63" s="31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="6:23" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O64" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="P64" s="36">
+        <v>9</v>
+      </c>
+      <c r="Q64" s="37">
+        <v>10</v>
+      </c>
+      <c r="R64" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="U64" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="V64" s="41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="65" spans="15:22" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O65" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="P65" s="36">
+        <v>11</v>
+      </c>
+      <c r="Q65" s="37">
+        <v>12</v>
+      </c>
+      <c r="R65" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="U65" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="V65" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="66" spans="15:22" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="O66" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="P66" s="36">
+        <v>13</v>
+      </c>
+      <c r="Q66" s="37">
+        <v>14</v>
+      </c>
+      <c r="R66" s="31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="15:22" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="O67" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="P67" s="36">
+        <v>15</v>
+      </c>
+      <c r="Q67" s="37">
+        <v>16</v>
+      </c>
+      <c r="R67" s="43" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="68" spans="15:22" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O68" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="P68" s="36">
+        <v>17</v>
+      </c>
+      <c r="Q68" s="37">
+        <v>18</v>
+      </c>
+      <c r="R68" s="45" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="15:22" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O69" s="26"/>
+      <c r="P69" s="36">
+        <v>19</v>
+      </c>
+      <c r="Q69" s="37">
+        <v>20</v>
+      </c>
+      <c r="R69" s="31"/>
+    </row>
+    <row r="70" spans="15:22" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O70" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="P70" s="36">
+        <v>21</v>
+      </c>
+      <c r="Q70" s="37">
+        <v>22</v>
+      </c>
+      <c r="R70" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="15:22" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O71" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="P71" s="36">
+        <v>23</v>
+      </c>
+      <c r="Q71" s="37">
+        <v>24</v>
+      </c>
+      <c r="R71" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="72" spans="15:22" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O72" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="P72" s="36">
+        <v>25</v>
+      </c>
+      <c r="Q72" s="37">
+        <v>26</v>
+      </c>
+      <c r="R72" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="15:22" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O73" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="P73" s="36">
+        <v>27</v>
+      </c>
+      <c r="Q73" s="37">
+        <v>28</v>
+      </c>
+      <c r="R73" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74" spans="15:22" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O74" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="P74" s="36">
+        <v>29</v>
+      </c>
+      <c r="Q74" s="37">
+        <v>30</v>
+      </c>
+      <c r="R74" s="32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="75" spans="15:22" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O75" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="P75" s="36">
+        <v>31</v>
+      </c>
+      <c r="Q75" s="37">
+        <v>32</v>
+      </c>
+      <c r="R75" s="31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="15:22" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O76" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="P76" s="36">
+        <v>33</v>
+      </c>
+      <c r="Q76" s="37">
+        <v>34</v>
+      </c>
+      <c r="R76" s="31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="15:22" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O77" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="P77" s="36">
+        <v>35</v>
+      </c>
+      <c r="Q77" s="37">
+        <v>36</v>
+      </c>
+      <c r="R77" s="31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="78" spans="15:22" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="O78" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="P78" s="36">
+        <v>37</v>
+      </c>
+      <c r="Q78" s="37">
+        <v>38</v>
+      </c>
+      <c r="R78" s="31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="15:22" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="O79" s="29"/>
+      <c r="P79" s="38">
+        <v>39</v>
+      </c>
+      <c r="Q79" s="39">
+        <v>40</v>
+      </c>
+      <c r="R79" s="33"/>
+    </row>
+    <row r="80" spans="15:22" x14ac:dyDescent="0.4">
+      <c r="P80" s="23"/>
+      <c r="Q80" s="23"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="P58:Q58"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>